<commit_message>
wip autoeval doc de projet
</commit_message>
<xml_diff>
--- a/doc/Documents autres évaluation/EvalDoc_samuel-auto-eval.xlsx
+++ b/doc/Documents autres évaluation/EvalDoc_samuel-auto-eval.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="4320" windowWidth="21600" windowHeight="11385" tabRatio="500"/>
+    <workbookView xWindow="3375" yWindow="4320" windowWidth="21600" windowHeight="11385" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
   <si>
     <t>Divers</t>
   </si>
@@ -246,9 +246,6 @@
     <t>à faire à la fin.</t>
   </si>
   <si>
-    <t>ca ma lair bon ?</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -259,6 +256,12 @@
   </si>
   <si>
     <t>why slt  quand presque total??</t>
+  </si>
+  <si>
+    <t>pk on fait el proj. Pour apprendre à coder pour réaliser un projet en entier soi meme</t>
+  </si>
+  <si>
+    <t>date de fin de sprint à rajouter !!</t>
   </si>
 </sst>
 </file>
@@ -283,7 +286,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,6 +305,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -315,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -341,6 +350,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -672,7 +684,7 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2">
@@ -680,26 +692,26 @@
       </c>
       <c r="E2" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="F2" s="8">
         <f ca="1">MROUND(2*RAND()+3,0.5)</f>
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="G2" s="8">
         <f ca="1">MROUND(1*RAND()+3,0.5)</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="H2" s="8">
         <f ca="1">MROUND(5*RAND()+1,0.5)</f>
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2">
@@ -707,26 +719,26 @@
       </c>
       <c r="E3" s="8">
         <f t="shared" ref="E3" ca="1" si="0">MROUND(3*RAND()+3,0.5)</f>
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="F3" s="8">
         <f t="shared" ref="F3:F25" ca="1" si="1">MROUND(2*RAND()+3,0.5)</f>
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="G3" s="8">
         <f t="shared" ref="G3:G25" ca="1" si="2">MROUND(1*RAND()+3,0.5)</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="H3" s="8">
         <f t="shared" ref="H3:H25" ca="1" si="3">MROUND(5*RAND()+1,0.5)</f>
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2">
@@ -752,7 +764,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="2">
@@ -781,7 +793,7 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2">
@@ -807,7 +819,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2">
@@ -833,7 +845,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2">
@@ -859,7 +871,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="2">
@@ -896,11 +908,11 @@
       </c>
       <c r="E10" s="8">
         <f t="shared" ref="E10:E20" ca="1" si="4">MROUND(3*RAND()+3,0.5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F10" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="G10" s="8">
         <f t="shared" ca="1" si="2"/>
@@ -908,14 +920,17 @@
       </c>
       <c r="H10" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="I10" s="8">
         <v>4</v>
       </c>
+      <c r="J10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="2">
@@ -923,7 +938,7 @@
       </c>
       <c r="E11" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="F11" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -931,18 +946,18 @@
       </c>
       <c r="G11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H11" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="I11" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="2">
@@ -950,11 +965,11 @@
       </c>
       <c r="E12" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="F12" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="G12" s="8">
         <f t="shared" ca="1" si="2"/>
@@ -962,14 +977,14 @@
       </c>
       <c r="H12" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="I12" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="2">
@@ -981,15 +996,15 @@
       </c>
       <c r="F13" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="G13" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="H13" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="I13" s="8">
         <v>5</v>
@@ -999,7 +1014,7 @@
       <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2">
@@ -1007,19 +1022,19 @@
       </c>
       <c r="E14" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="F14" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="H14" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="I14" s="8">
         <v>4</v>
@@ -1029,7 +1044,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="2">
@@ -1037,19 +1052,19 @@
       </c>
       <c r="E15" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="F15" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I15" s="8">
         <v>5</v>
@@ -1059,7 +1074,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="2">
@@ -1067,7 +1082,7 @@
       </c>
       <c r="E16" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -1075,18 +1090,18 @@
       </c>
       <c r="G16" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="H16" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I16" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2">
@@ -1094,11 +1109,11 @@
       </c>
       <c r="E17" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" ca="1" si="2"/>
@@ -1106,7 +1121,7 @@
       </c>
       <c r="H17" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="I17" s="8">
         <v>4</v>
@@ -1116,7 +1131,7 @@
       <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2">
@@ -1124,26 +1139,26 @@
       </c>
       <c r="E18" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F18" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="G18" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H18" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="J18" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="2">
@@ -1151,26 +1166,26 @@
       </c>
       <c r="E19" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="G19" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H19" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="J19" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="2">
@@ -1190,14 +1205,14 @@
       </c>
       <c r="H20" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="J20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="2">
@@ -1226,7 +1241,7 @@
       <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="2">
@@ -1234,26 +1249,26 @@
       </c>
       <c r="E22" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="F22" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G22" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H22" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J22" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="2">
@@ -1261,19 +1276,19 @@
       </c>
       <c r="E23" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="G23" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="H23" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="J23" t="s">
         <v>59</v>
@@ -1291,11 +1306,11 @@
       </c>
       <c r="E24" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="F24" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="G24" s="8">
         <f t="shared" ca="1" si="2"/>
@@ -1303,7 +1318,7 @@
       </c>
       <c r="H24" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J24" t="s">
         <v>60</v>
@@ -1321,11 +1336,11 @@
       </c>
       <c r="E25" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F25" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="G25" s="8">
         <f t="shared" ca="1" si="2"/>
@@ -1333,17 +1348,17 @@
       </c>
       <c r="H25" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="J25" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="2">
@@ -1365,17 +1380,17 @@
         <v>6</v>
       </c>
       <c r="I26" t="s">
+        <v>61</v>
+      </c>
+      <c r="J26" t="s">
         <v>62</v>
-      </c>
-      <c r="J26" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="2">
@@ -1401,7 +1416,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C28" s="2">
@@ -1427,7 +1442,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="2">
@@ -1449,11 +1464,11 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="2">
@@ -1510,7 +1525,7 @@
       </c>
       <c r="E34" s="8">
         <f ca="1">MROUND(SUMPRODUCT($C2:$C31,E2:E31)/(SUM($C2:$C31)*6)*5+1,0.1)</f>
-        <v>4.9000000000000004</v>
+        <v>4.8000000000000007</v>
       </c>
       <c r="F34" s="8">
         <f t="shared" ref="F34:G34" ca="1" si="5">MROUND(SUMPRODUCT($C2:$C31,F2:F31)/(SUM($C2:$C31)*6)*5+1,0.1)</f>
@@ -1518,11 +1533,11 @@
       </c>
       <c r="G34" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>3.5</v>
+        <v>3.4000000000000004</v>
       </c>
       <c r="H34" s="8">
         <f ca="1">MROUND(SUMPRODUCT($C2:$C31,H2:H31)/(SUM($C2:$C31)*6)*5+1,0.1)</f>
-        <v>3.8000000000000003</v>
+        <v>3.9000000000000004</v>
       </c>
       <c r="I34" s="8">
         <f>MROUND(SUMPRODUCT($C2:$C31,I2:I31)/(SUM($C2:$C31)*6)*5+1,0.1)</f>
@@ -1554,7 +1569,7 @@
         <v>2.5</v>
       </c>
       <c r="J35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
très petite optimisation. aucune influence. release Version 1.3
</commit_message>
<xml_diff>
--- a/doc/Documents autres évaluation/EvalDoc_samuel-auto-eval.xlsx
+++ b/doc/Documents autres évaluation/EvalDoc_samuel-auto-eval.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_Samuel_01\Documents\GitHub\BN-SRD-Bataille-Navale\doc\Documents autres évaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D63928-332F-46C2-A54C-0D12491E15B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08319594-2E4E-4BFD-B24E-BE84C0AA42CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2445" yWindow="2040" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t>Divers</t>
   </si>
@@ -235,9 +235,6 @@
     <t>idem</t>
   </si>
   <si>
-    <t>assurer que complet…</t>
-  </si>
-  <si>
     <t>à checker  fini</t>
   </si>
   <si>
@@ -250,25 +247,16 @@
     <t>?</t>
   </si>
   <si>
-    <t>sdc + carrel + …?</t>
-  </si>
-  <si>
     <t>à checker  à la fin</t>
   </si>
   <si>
-    <t>why slt  quand presque total??</t>
-  </si>
-  <si>
-    <t>pk on fait el proj. Pour apprendre à coder pour réaliser un projet en entier soi meme</t>
-  </si>
-  <si>
     <t>date de fin de sprint à rajouter !!</t>
   </si>
   <si>
     <t>autre ???</t>
   </si>
   <si>
-    <t>d'autres avec grille externes?</t>
+    <t>sdc + carrel + code carrel carac semigraphics</t>
   </si>
 </sst>
 </file>
@@ -643,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -705,15 +693,15 @@
       </c>
       <c r="F2" s="8">
         <f ca="1">MROUND(2*RAND()+3,0.5)</f>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="G2" s="8">
         <f ca="1">MROUND(1*RAND()+3,0.5)</f>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="H2" s="8">
         <f ca="1">MROUND(5*RAND()+1,0.5)</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -728,19 +716,19 @@
       </c>
       <c r="E3" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="F3" s="8">
         <f t="shared" ref="F3:F25" ca="1" si="0">MROUND(2*RAND()+3,0.5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" s="8">
         <f t="shared" ref="G3:G25" ca="1" si="1">MROUND(1*RAND()+3,0.5)</f>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="H3" s="8">
         <f t="shared" ref="H3:H25" ca="1" si="2">MROUND(5*RAND()+1,0.5)</f>
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -917,25 +905,22 @@
       </c>
       <c r="E10" s="8">
         <f t="shared" ref="E10:E20" ca="1" si="3">MROUND(3*RAND()+3,0.5)</f>
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="F10" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G10" s="8">
         <f ca="1">MROUND(1*RAND()+3,0.5)</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H10" s="8">
         <f ca="1">MROUND(5*RAND()+1,0.5)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I10" s="8">
         <v>4</v>
-      </c>
-      <c r="J10" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -947,7 +932,7 @@
       </c>
       <c r="E11" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="8">
         <f t="shared" ca="1" si="0"/>
@@ -955,11 +940,11 @@
       </c>
       <c r="G11" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="I11" s="8">
         <v>2</v>
@@ -974,19 +959,19 @@
       </c>
       <c r="E12" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F12" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="G12" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="I12" s="8">
         <v>4</v>
@@ -1001,19 +986,19 @@
       </c>
       <c r="E13" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="G13" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="H13" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5</v>
+        <v>5.5</v>
       </c>
       <c r="I13" s="8">
         <v>5</v>
@@ -1031,11 +1016,11 @@
       </c>
       <c r="E14" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="F14" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -1043,7 +1028,7 @@
       </c>
       <c r="H14" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="I14" s="8">
         <v>4</v>
@@ -1061,15 +1046,15 @@
       </c>
       <c r="E15" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="F15" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" ca="1" si="2"/>
@@ -1091,19 +1076,19 @@
       </c>
       <c r="E16" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="G16" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H16" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I16" s="8">
         <v>3</v>
@@ -1118,7 +1103,7 @@
       </c>
       <c r="E17" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" ca="1" si="0"/>
@@ -1130,7 +1115,7 @@
       </c>
       <c r="H17" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="I17" s="8">
         <v>4</v>
@@ -1148,19 +1133,19 @@
       </c>
       <c r="E18" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F18" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G18" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H18" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="I18" s="8">
         <v>4</v>
@@ -1178,7 +1163,7 @@
       </c>
       <c r="E19" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="F19" s="8">
         <f t="shared" ca="1" si="0"/>
@@ -1186,17 +1171,14 @@
       </c>
       <c r="G19" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="H19" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I19" s="8">
         <v>5</v>
-      </c>
-      <c r="J19" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1208,7 +1190,7 @@
       </c>
       <c r="E20" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="F20" s="8">
         <f t="shared" ca="1" si="0"/>
@@ -1216,15 +1198,13 @@
       </c>
       <c r="G20" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="H20" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>68</v>
-      </c>
+        <v>5.5</v>
+      </c>
+      <c r="I20" s="8"/>
       <c r="J20" t="s">
         <v>55</v>
       </c>
@@ -1267,11 +1247,11 @@
       </c>
       <c r="E22" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F22" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G22" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -1282,7 +1262,7 @@
         <v>4.5</v>
       </c>
       <c r="J22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1294,7 +1274,7 @@
       </c>
       <c r="E23" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" ca="1" si="0"/>
@@ -1306,10 +1286,10 @@
       </c>
       <c r="H23" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1324,7 +1304,7 @@
       </c>
       <c r="E24" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="F24" s="8">
         <f t="shared" ca="1" si="0"/>
@@ -1332,14 +1312,14 @@
       </c>
       <c r="G24" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="H24" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1354,25 +1334,25 @@
       </c>
       <c r="E25" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="F25" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="G25" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H25" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="J25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="M25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1401,10 +1381,10 @@
         <v>6</v>
       </c>
       <c r="I26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J26" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1433,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
@@ -1485,7 +1465,7 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
@@ -1540,7 +1520,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>48</v>
       </c>
@@ -1550,7 +1530,7 @@
       </c>
       <c r="F34" s="8">
         <f t="shared" ref="F34:G34" ca="1" si="4">MROUND(SUMPRODUCT($C2:$C31,F2:F31)/(SUM($C2:$C31)*6)*5+1,0.1)</f>
-        <v>4.7</v>
+        <v>4.5</v>
       </c>
       <c r="G34" s="8">
         <f t="shared" ca="1" si="4"/>
@@ -1558,14 +1538,14 @@
       </c>
       <c r="H34" s="8">
         <f ca="1">MROUND(SUMPRODUCT($C2:$C31,H2:H31)/(SUM($C2:$C31)*6)*5+1,0.1)</f>
-        <v>3.8000000000000003</v>
+        <v>4</v>
       </c>
       <c r="I34" s="8">
         <f>MROUND(SUMPRODUCT($C2:$C31,I2:I31)/(SUM($C2:$C31)*6)*5+1,0.1)</f>
         <v>3.3000000000000003</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>49</v>
       </c>
@@ -1588,9 +1568,6 @@
       <c r="I35" s="8">
         <f>MROUND(SUMPRODUCT($C2:$C31,I2:I31)/(SUM($C2:$C31)*6)*5+1,0.5)</f>
         <v>3.5</v>
-      </c>
-      <c r="J35" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documentation de projet terminée pour le sprint 5
</commit_message>
<xml_diff>
--- a/doc/Documents autres évaluation/EvalDoc_samuel-auto-eval.xlsx
+++ b/doc/Documents autres évaluation/EvalDoc_samuel-auto-eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_Samuel_01\Documents\GitHub\BN-SRD-Bataille-Navale\doc\Documents autres évaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08319594-2E4E-4BFD-B24E-BE84C0AA42CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D035268A-0272-40B4-969A-40A15D6CCDE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="2040" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10080" yWindow="1410" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
   <si>
     <t>Divers</t>
   </si>
@@ -220,43 +220,19 @@
     <t>Samuel check perso</t>
   </si>
   <si>
-    <t>à voir</t>
-  </si>
-  <si>
-    <t>a voir</t>
-  </si>
-  <si>
-    <t>à completer valeur</t>
-  </si>
-  <si>
-    <t>à completer. Voir pour les grilles à placer ou choisir…</t>
-  </si>
-  <si>
     <t>idem</t>
   </si>
   <si>
-    <t>à checker  fini</t>
-  </si>
-  <si>
-    <t>????????????????????????????????????????????????????</t>
-  </si>
-  <si>
-    <t>à faire à la fin.</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
     <t>à checker  à la fin</t>
   </si>
   <si>
-    <t>date de fin de sprint à rajouter !!</t>
-  </si>
-  <si>
-    <t>autre ???</t>
-  </si>
-  <si>
-    <t>sdc + carrel + code carrel carac semigraphics</t>
+    <t>o</t>
+  </si>
+  <si>
+    <t>o=OK</t>
   </si>
 </sst>
 </file>
@@ -629,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -676,6 +652,9 @@
       <c r="I1" s="7" t="s">
         <v>51</v>
       </c>
+      <c r="J1" s="7" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -689,11 +668,11 @@
       </c>
       <c r="E2" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="F2" s="8">
         <f ca="1">MROUND(2*RAND()+3,0.5)</f>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="G2" s="8">
         <f ca="1">MROUND(1*RAND()+3,0.5)</f>
@@ -701,10 +680,13 @@
       </c>
       <c r="H2" s="8">
         <f ca="1">MROUND(5*RAND()+1,0.5)</f>
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="I2">
         <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -716,11 +698,11 @@
       </c>
       <c r="E3" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="8">
         <f t="shared" ref="F3:F25" ca="1" si="0">MROUND(2*RAND()+3,0.5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G3" s="8">
         <f t="shared" ref="G3:G25" ca="1" si="1">MROUND(1*RAND()+3,0.5)</f>
@@ -728,10 +710,13 @@
       </c>
       <c r="H3" s="8">
         <f t="shared" ref="H3:H25" ca="1" si="2">MROUND(5*RAND()+1,0.5)</f>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -759,6 +744,9 @@
       <c r="I4" s="8">
         <v>6</v>
       </c>
+      <c r="J4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
@@ -785,6 +773,9 @@
       <c r="I5" s="8">
         <v>6</v>
       </c>
+      <c r="J5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -814,6 +805,9 @@
       <c r="I6" s="8">
         <v>6</v>
       </c>
+      <c r="J6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -840,6 +834,9 @@
       <c r="I7" s="8">
         <v>6</v>
       </c>
+      <c r="J7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
@@ -866,6 +863,9 @@
       <c r="I8" s="8">
         <v>6</v>
       </c>
+      <c r="J8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -892,6 +892,9 @@
       <c r="I9" s="8">
         <v>6</v>
       </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -905,22 +908,25 @@
       </c>
       <c r="E10" s="8">
         <f t="shared" ref="E10:E20" ca="1" si="3">MROUND(3*RAND()+3,0.5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="G10" s="8">
         <f ca="1">MROUND(1*RAND()+3,0.5)</f>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="H10" s="8">
         <f ca="1">MROUND(5*RAND()+1,0.5)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I10" s="8">
         <v>4</v>
+      </c>
+      <c r="J10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -940,14 +946,17 @@
       </c>
       <c r="G11" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>5.5</v>
+        <v>1.5</v>
       </c>
       <c r="I11" s="8">
         <v>2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -963,18 +972,21 @@
       </c>
       <c r="F12" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="G12" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="I12" s="8">
         <v>4</v>
+      </c>
+      <c r="J12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -990,18 +1002,21 @@
       </c>
       <c r="F13" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="G13" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H13" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I13" s="8">
         <v>5</v>
+      </c>
+      <c r="J13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1016,11 +1031,11 @@
       </c>
       <c r="E14" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F14" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -1028,13 +1043,13 @@
       </c>
       <c r="H14" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="I14" s="8">
         <v>4</v>
       </c>
       <c r="J14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1046,25 +1061,25 @@
       </c>
       <c r="E15" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="F15" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="I15" s="8">
         <v>5</v>
       </c>
       <c r="J15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1076,11 +1091,11 @@
       </c>
       <c r="E16" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="G16" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -1088,13 +1103,16 @@
       </c>
       <c r="H16" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I16" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>23</v>
       </c>
@@ -1103,15 +1121,15 @@
       </c>
       <c r="E17" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="H17" s="8">
         <f t="shared" ca="1" si="2"/>
@@ -1120,8 +1138,11 @@
       <c r="I17" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1133,28 +1154,28 @@
       </c>
       <c r="E18" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="F18" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G18" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="H18" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>5.5</v>
+        <v>1.5</v>
       </c>
       <c r="I18" s="8">
         <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>26</v>
       </c>
@@ -1163,25 +1184,28 @@
       </c>
       <c r="E19" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="F19" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="G19" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H19" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="I19" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
         <v>27</v>
       </c>
@@ -1190,26 +1214,26 @@
       </c>
       <c r="E20" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="F20" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="G20" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="H20" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="I20" s="8"/>
       <c r="J20" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>28</v>
       </c>
@@ -1234,8 +1258,11 @@
       <c r="I21" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1247,11 +1274,11 @@
       </c>
       <c r="E22" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F22" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G22" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -1259,13 +1286,13 @@
       </c>
       <c r="H22" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="J22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>30</v>
       </c>
@@ -1274,11 +1301,11 @@
       </c>
       <c r="E23" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="G23" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -1286,13 +1313,13 @@
       </c>
       <c r="H23" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="J23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1304,25 +1331,25 @@
       </c>
       <c r="E24" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="F24" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G24" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H24" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>3</v>
       </c>
       <c r="J24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1334,11 +1361,11 @@
       </c>
       <c r="E25" s="8">
         <f ca="1">MROUND(3*RAND()+3,0.5)</f>
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="F25" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="G25" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -1346,16 +1373,13 @@
       </c>
       <c r="H25" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J25" t="s">
-        <v>62</v>
-      </c>
-      <c r="M25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1381,13 +1405,13 @@
         <v>6</v>
       </c>
       <c r="I26" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="J26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1413,10 +1437,10 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>42</v>
       </c>
@@ -1441,8 +1465,11 @@
       <c r="I28" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>2</v>
       </c>
@@ -1465,10 +1492,10 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
         <v>3</v>
       </c>
@@ -1491,10 +1518,10 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>37</v>
       </c>
@@ -1517,7 +1544,7 @@
         <v>6</v>
       </c>
       <c r="J31" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -1526,7 +1553,7 @@
       </c>
       <c r="E34" s="8">
         <f ca="1">MROUND(SUMPRODUCT($C2:$C31,E2:E31)/(SUM($C2:$C31)*6)*5+1,0.1)</f>
-        <v>4.9000000000000004</v>
+        <v>4.8000000000000007</v>
       </c>
       <c r="F34" s="8">
         <f t="shared" ref="F34:G34" ca="1" si="4">MROUND(SUMPRODUCT($C2:$C31,F2:F31)/(SUM($C2:$C31)*6)*5+1,0.1)</f>
@@ -1534,11 +1561,11 @@
       </c>
       <c r="G34" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>3.5</v>
+        <v>3.4000000000000004</v>
       </c>
       <c r="H34" s="8">
         <f ca="1">MROUND(SUMPRODUCT($C2:$C31,H2:H31)/(SUM($C2:$C31)*6)*5+1,0.1)</f>
-        <v>4</v>
+        <v>3.9000000000000004</v>
       </c>
       <c r="I34" s="8">
         <f>MROUND(SUMPRODUCT($C2:$C31,I2:I31)/(SUM($C2:$C31)*6)*5+1,0.1)</f>

</xml_diff>